<commit_message>
Statement collection create and validate the saved data in grid. Data driven using data provider,
</commit_message>
<xml_diff>
--- a/VansalesProject/Excel/TestData.xlsx
+++ b/VansalesProject/Excel/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="23955" windowHeight="10815" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="23955" windowHeight="10815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>UserName</t>
   </si>
@@ -45,16 +45,25 @@
     <t>StatementNo</t>
   </si>
   <si>
-    <t>Test outlet</t>
-  </si>
-  <si>
-    <t>St2235</t>
-  </si>
-  <si>
     <t>654645</t>
   </si>
   <si>
     <t>6466546</t>
+  </si>
+  <si>
+    <t>MZ-0004</t>
+  </si>
+  <si>
+    <t>STA00006</t>
+  </si>
+  <si>
+    <t>MZ-0005</t>
+  </si>
+  <si>
+    <t>STA00007</t>
+  </si>
+  <si>
+    <t>CollectAmt</t>
   </si>
 </sst>
 </file>
@@ -423,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -439,10 +448,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -460,10 +469,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -472,20 +481,37 @@
     <col min="2" max="2" width="23.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>